<commit_message>
final all bug fix
</commit_message>
<xml_diff>
--- a/assets/weightmissmatch_import/weight_missmatch_import.xlsx
+++ b/assets/weightmissmatch_import/weight_missmatch_import.xlsx
@@ -19,24 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Awbno</t>
   </si>
   <si>
     <t>Actualweight</t>
-  </si>
-  <si>
-    <t>SF166804397SHS</t>
-  </si>
-  <si>
-    <t>SF164479604SHS</t>
-  </si>
-  <si>
-    <t>SF166827773SHS</t>
-  </si>
-  <si>
-    <t>SF166828149SHS</t>
   </si>
 </sst>
 </file>
@@ -354,15 +342,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -375,38 +363,15 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
+      <c r="A2">
+        <v>4714411638593</v>
       </c>
       <c r="B2">
-        <v>6.8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>2.4500000000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>